<commit_message>
Add OrderedDistribution to model
</commit_message>
<xml_diff>
--- a/image/evidence.xlsx
+++ b/image/evidence.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3147" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="341">
   <si>
     <t>Path</t>
   </si>
@@ -968,10 +968,19 @@
     <t>Evidence.population.evidenceVariable.statisticCollection.statistic</t>
   </si>
   <si>
-    <t>The statistic value(s)</t>
-  </si>
-  <si>
-    <t>The statistic value(s).</t>
+    <t>The statistic value(s) - sb type Statistic</t>
+  </si>
+  <si>
+    <t>The statistic value(s) - sb type Statistic.</t>
+  </si>
+  <si>
+    <t>Evidence.population.evidenceVariable.distribution</t>
+  </si>
+  <si>
+    <t>Ordered distribution - sb type OrderedDistribution</t>
+  </si>
+  <si>
+    <t>Ordered distribution - sb type OrderedDistribution.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.nestedVariable</t>
@@ -1192,7 +1201,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM91"/>
+  <dimension ref="A1:AM92"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -8767,7 +8776,7 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="K69" t="s" s="2">
         <v>310</v>
@@ -8836,7 +8845,7 @@
         <v>40</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>40</v>
@@ -8864,7 +8873,7 @@
         <v>41</v>
       </c>
       <c r="F70" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G70" t="s" s="2">
         <v>40</v>
@@ -8876,13 +8885,13 @@
         <v>40</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>186</v>
+        <v>314</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -8933,19 +8942,19 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>187</v>
+        <v>312</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG70" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH70" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>40</v>
+        <v>183</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>40</v>
@@ -8954,7 +8963,7 @@
         <v>40</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>188</v>
+        <v>40</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>40</v>
@@ -8962,18 +8971,18 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>40</v>
@@ -8985,17 +8994,15 @@
         <v>40</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>96</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="M71" s="2"/>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
         <v>40</v>
@@ -9044,13 +9051,13 @@
         <v>40</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH71" t="s" s="2">
         <v>40</v>
@@ -9073,11 +9080,11 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" t="s" s="2">
@@ -9090,26 +9097,24 @@
         <v>40</v>
       </c>
       <c r="H72" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I72" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J72" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>194</v>
+        <v>94</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M72" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="N72" t="s" s="2">
-        <v>101</v>
-      </c>
+      <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
         <v>40</v>
       </c>
@@ -9157,7 +9162,7 @@
         <v>40</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>41</v>
@@ -9178,7 +9183,7 @@
         <v>40</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>40</v>
@@ -9186,39 +9191,43 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H73" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>278</v>
+        <v>194</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="M73" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N73" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="O73" t="s" s="2">
         <v>40</v>
       </c>
@@ -9266,13 +9275,13 @@
         <v>40</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>315</v>
+        <v>196</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>40</v>
@@ -9287,7 +9296,7 @@
         <v>40</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>40</v>
@@ -9295,7 +9304,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9306,7 +9315,7 @@
         <v>41</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>40</v>
@@ -9318,13 +9327,13 @@
         <v>40</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>219</v>
+        <v>278</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>220</v>
+        <v>279</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9375,13 +9384,13 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG74" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH74" t="s" s="2">
         <v>40</v>
@@ -9404,7 +9413,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9415,7 +9424,7 @@
         <v>41</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>40</v>
@@ -9427,13 +9436,13 @@
         <v>40</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>67</v>
+        <v>218</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>282</v>
+        <v>219</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>283</v>
+        <v>220</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -9460,13 +9469,13 @@
         <v>40</v>
       </c>
       <c r="W75" t="s" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="X75" t="s" s="2">
-        <v>284</v>
+        <v>40</v>
       </c>
       <c r="Y75" t="s" s="2">
-        <v>285</v>
+        <v>40</v>
       </c>
       <c r="Z75" t="s" s="2">
         <v>40</v>
@@ -9484,13 +9493,13 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>40</v>
@@ -9513,7 +9522,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9521,7 +9530,7 @@
       </c>
       <c r="D76" s="2"/>
       <c r="E76" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F76" t="s" s="2">
         <v>48</v>
@@ -9533,16 +9542,16 @@
         <v>40</v>
       </c>
       <c r="I76" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>287</v>
+        <v>67</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9569,13 +9578,13 @@
         <v>40</v>
       </c>
       <c r="W76" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="X76" t="s" s="2">
-        <v>40</v>
+        <v>284</v>
       </c>
       <c r="Y76" t="s" s="2">
-        <v>40</v>
+        <v>285</v>
       </c>
       <c r="Z76" t="s" s="2">
         <v>40</v>
@@ -9593,10 +9602,10 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>48</v>
@@ -9622,7 +9631,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9630,10 +9639,10 @@
       </c>
       <c r="D77" s="2"/>
       <c r="E77" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>40</v>
@@ -9642,16 +9651,16 @@
         <v>40</v>
       </c>
       <c r="I77" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>180</v>
+        <v>287</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -9702,19 +9711,19 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AG77" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="AJ77" t="s" s="2">
         <v>40</v>
@@ -9731,7 +9740,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9742,7 +9751,7 @@
         <v>41</v>
       </c>
       <c r="F78" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G78" t="s" s="2">
         <v>40</v>
@@ -9754,13 +9763,13 @@
         <v>40</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>185</v>
+        <v>291</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>186</v>
+        <v>292</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -9811,19 +9820,19 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>187</v>
+        <v>322</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG78" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH78" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>40</v>
+        <v>183</v>
       </c>
       <c r="AJ78" t="s" s="2">
         <v>40</v>
@@ -9832,7 +9841,7 @@
         <v>40</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>188</v>
+        <v>40</v>
       </c>
       <c r="AM78" t="s" s="2">
         <v>40</v>
@@ -9840,18 +9849,18 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G79" t="s" s="2">
         <v>40</v>
@@ -9863,17 +9872,15 @@
         <v>40</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>96</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="M79" s="2"/>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>40</v>
@@ -9922,13 +9929,13 @@
         <v>40</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG79" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH79" t="s" s="2">
         <v>40</v>
@@ -9951,11 +9958,11 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
@@ -9968,26 +9975,24 @@
         <v>40</v>
       </c>
       <c r="H80" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J80" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>194</v>
+        <v>94</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M80" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="N80" t="s" s="2">
-        <v>101</v>
-      </c>
+      <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
         <v>40</v>
       </c>
@@ -10035,7 +10040,7 @@
         <v>40</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>41</v>
@@ -10056,7 +10061,7 @@
         <v>40</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="AM80" t="s" s="2">
         <v>40</v>
@@ -10064,39 +10069,43 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G81" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H81" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I81" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>297</v>
+        <v>194</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="M81" s="2"/>
-      <c r="N81" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="M81" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="O81" t="s" s="2">
         <v>40</v>
       </c>
@@ -10144,13 +10153,13 @@
         <v>40</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>323</v>
+        <v>196</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG81" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH81" t="s" s="2">
         <v>40</v>
@@ -10165,7 +10174,7 @@
         <v>40</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="AM81" t="s" s="2">
         <v>40</v>
@@ -10173,7 +10182,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10184,7 +10193,7 @@
         <v>41</v>
       </c>
       <c r="F82" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G82" t="s" s="2">
         <v>40</v>
@@ -10196,13 +10205,13 @@
         <v>40</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>219</v>
+        <v>297</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>220</v>
+        <v>298</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -10253,13 +10262,13 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG82" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH82" t="s" s="2">
         <v>40</v>
@@ -10282,7 +10291,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10293,7 +10302,7 @@
         <v>41</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>40</v>
@@ -10305,13 +10314,13 @@
         <v>40</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>301</v>
+        <v>219</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>302</v>
+        <v>220</v>
       </c>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -10338,13 +10347,13 @@
         <v>40</v>
       </c>
       <c r="W83" t="s" s="2">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>226</v>
+        <v>40</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>227</v>
+        <v>40</v>
       </c>
       <c r="Z83" t="s" s="2">
         <v>40</v>
@@ -10362,13 +10371,13 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH83" t="s" s="2">
         <v>40</v>
@@ -10391,7 +10400,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10417,10 +10426,10 @@
         <v>222</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -10450,10 +10459,10 @@
         <v>225</v>
       </c>
       <c r="X84" t="s" s="2">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="Z84" t="s" s="2">
         <v>40</v>
@@ -10471,7 +10480,7 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
@@ -10500,7 +10509,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10511,7 +10520,7 @@
         <v>41</v>
       </c>
       <c r="F85" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>40</v>
@@ -10523,13 +10532,13 @@
         <v>40</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -10556,13 +10565,13 @@
         <v>40</v>
       </c>
       <c r="W85" t="s" s="2">
-        <v>40</v>
+        <v>225</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>40</v>
+        <v>231</v>
       </c>
       <c r="Y85" t="s" s="2">
-        <v>40</v>
+        <v>232</v>
       </c>
       <c r="Z85" t="s" s="2">
         <v>40</v>
@@ -10580,19 +10589,19 @@
         <v>40</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH85" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>183</v>
+        <v>40</v>
       </c>
       <c r="AJ85" t="s" s="2">
         <v>40</v>
@@ -10620,7 +10629,7 @@
         <v>41</v>
       </c>
       <c r="F86" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G86" t="s" s="2">
         <v>40</v>
@@ -10632,13 +10641,13 @@
         <v>40</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>185</v>
+        <v>331</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>186</v>
+        <v>332</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -10689,19 +10698,19 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>187</v>
+        <v>330</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG86" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH86" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>40</v>
+        <v>183</v>
       </c>
       <c r="AJ86" t="s" s="2">
         <v>40</v>
@@ -10710,7 +10719,7 @@
         <v>40</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>188</v>
+        <v>40</v>
       </c>
       <c r="AM86" t="s" s="2">
         <v>40</v>
@@ -10718,18 +10727,18 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F87" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G87" t="s" s="2">
         <v>40</v>
@@ -10741,17 +10750,15 @@
         <v>40</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="M87" t="s" s="2">
-        <v>96</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="M87" s="2"/>
       <c r="N87" s="2"/>
       <c r="O87" t="s" s="2">
         <v>40</v>
@@ -10800,13 +10807,13 @@
         <v>40</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AF87" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG87" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="AH87" t="s" s="2">
         <v>40</v>
@@ -10829,11 +10836,11 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" t="s" s="2">
@@ -10846,26 +10853,24 @@
         <v>40</v>
       </c>
       <c r="H88" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="I88" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J88" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>194</v>
+        <v>94</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M88" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="N88" t="s" s="2">
-        <v>101</v>
-      </c>
+      <c r="N88" s="2"/>
       <c r="O88" t="s" s="2">
         <v>40</v>
       </c>
@@ -10913,7 +10918,7 @@
         <v>40</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>41</v>
@@ -10934,7 +10939,7 @@
         <v>40</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>90</v>
+        <v>188</v>
       </c>
       <c r="AM88" t="s" s="2">
         <v>40</v>
@@ -10942,39 +10947,43 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" t="s" s="2">
         <v>41</v>
       </c>
       <c r="F89" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G89" t="s" s="2">
         <v>40</v>
       </c>
       <c r="H89" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I89" t="s" s="2">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="J89" t="s" s="2">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>282</v>
+        <v>194</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="M89" s="2"/>
-      <c r="N89" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="M89" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="O89" t="s" s="2">
         <v>40</v>
       </c>
@@ -10998,13 +11007,13 @@
         <v>40</v>
       </c>
       <c r="W89" t="s" s="2">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="X89" t="s" s="2">
-        <v>284</v>
+        <v>40</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>285</v>
+        <v>40</v>
       </c>
       <c r="Z89" t="s" s="2">
         <v>40</v>
@@ -11022,13 +11031,13 @@
         <v>40</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>333</v>
+        <v>196</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AG89" t="s" s="2">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="AH89" t="s" s="2">
         <v>40</v>
@@ -11043,7 +11052,7 @@
         <v>40</v>
       </c>
       <c r="AL89" t="s" s="2">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="AM89" t="s" s="2">
         <v>40</v>
@@ -11051,7 +11060,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11059,7 +11068,7 @@
       </c>
       <c r="D90" s="2"/>
       <c r="E90" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F90" t="s" s="2">
         <v>48</v>
@@ -11071,16 +11080,16 @@
         <v>40</v>
       </c>
       <c r="I90" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>287</v>
+        <v>67</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>335</v>
+        <v>282</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>336</v>
+        <v>283</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -11107,13 +11116,13 @@
         <v>40</v>
       </c>
       <c r="W90" t="s" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="X90" t="s" s="2">
-        <v>40</v>
+        <v>284</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>40</v>
+        <v>285</v>
       </c>
       <c r="Z90" t="s" s="2">
         <v>40</v>
@@ -11131,10 +11140,10 @@
         <v>40</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>48</v>
@@ -11171,7 +11180,7 @@
         <v>48</v>
       </c>
       <c r="F91" t="s" s="2">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G91" t="s" s="2">
         <v>40</v>
@@ -11183,13 +11192,13 @@
         <v>49</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>162</v>
+        <v>287</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>307</v>
+        <v>338</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>308</v>
+        <v>339</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -11246,24 +11255,133 @@
         <v>48</v>
       </c>
       <c r="AG91" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL91" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM91" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F92" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="AH91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AK91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL91" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM91" t="s" s="2">
+      <c r="G92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I92" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J92" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="K92" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="L92" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE92" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="AF92" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AG92" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM92" t="s" s="2">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New Evidence resource w/ Statistic and OrderedDistribution data types
</commit_message>
<xml_diff>
--- a/image/evidence.xlsx
+++ b/image/evidence.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="343">
   <si>
     <t>Path</t>
   </si>
@@ -968,19 +968,27 @@
     <t>Evidence.population.evidenceVariable.statisticCollection.statistic</t>
   </si>
   <si>
-    <t>The statistic value(s) - sb type Statistic</t>
-  </si>
-  <si>
-    <t>The statistic value(s) - sb type Statistic.</t>
+    <t xml:space="preserve">Statistic
+</t>
+  </si>
+  <si>
+    <t>The statistic value(s)</t>
+  </si>
+  <si>
+    <t>The statistic value(s).</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.distribution</t>
   </si>
   <si>
-    <t>Ordered distribution - sb type OrderedDistribution</t>
-  </si>
-  <si>
-    <t>Ordered distribution - sb type OrderedDistribution.</t>
+    <t xml:space="preserve">OrderedDistribution
+</t>
+  </si>
+  <si>
+    <t>Ordered distribution</t>
+  </si>
+  <si>
+    <t>Ordered distribution.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.nestedVariable</t>
@@ -8667,13 +8675,13 @@
         <v>49</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>162</v>
+        <v>307</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8753,7 +8761,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8776,13 +8784,13 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>162</v>
+        <v>311</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -8833,7 +8841,7 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -8862,7 +8870,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8888,10 +8896,10 @@
         <v>180</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -8942,7 +8950,7 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -8971,7 +8979,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9080,7 +9088,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9191,7 +9199,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9304,7 +9312,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9384,7 +9392,7 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9413,7 +9421,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9493,7 +9501,7 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -9522,7 +9530,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9602,7 +9610,7 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -9631,7 +9639,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9711,7 +9719,7 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>48</v>
@@ -9740,7 +9748,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9820,7 +9828,7 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -9849,7 +9857,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9958,7 +9966,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10069,7 +10077,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10182,7 +10190,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10262,7 +10270,7 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10291,7 +10299,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10371,7 +10379,7 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
@@ -10400,7 +10408,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10480,7 +10488,7 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
@@ -10509,7 +10517,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10589,7 +10597,7 @@
         <v>40</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
@@ -10618,7 +10626,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10644,10 +10652,10 @@
         <v>180</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -10698,7 +10706,7 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -10727,7 +10735,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -10836,7 +10844,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -10947,7 +10955,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11060,7 +11068,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11140,7 +11148,7 @@
         <v>40</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>41</v>
@@ -11169,7 +11177,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11195,10 +11203,10 @@
         <v>287</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -11249,7 +11257,7 @@
         <v>40</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>48</v>
@@ -11278,7 +11286,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -11301,13 +11309,13 @@
         <v>49</v>
       </c>
       <c r="J92" t="s" s="2">
-        <v>162</v>
+        <v>307</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -11358,7 +11366,7 @@
         <v>40</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>48</v>

</xml_diff>

<commit_message>
Update evidence, statistic and ordereddistribution
</commit_message>
<xml_diff>
--- a/image/evidence.xlsx
+++ b/image/evidence.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3215" uniqueCount="341">
   <si>
     <t>Path</t>
   </si>
@@ -143,7 +143,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>A collection of evidence focused statistics</t>
+    <t>A collection of evidence focused statistics, considered a summary of evidence</t>
   </si>
   <si>
     <t>The representation of a collection of statistics for a given population and set of evidence variables.</t>
@@ -470,7 +470,7 @@
 </t>
   </si>
   <si>
-    <t>Use conte3xt</t>
+    <t>Use contetxt</t>
   </si>
   <si>
     <t>The content was developed with a focus and intent of supporting the contexts that are listed. These contexts may be general categories (gender, age, ...) or may be references to specific programs (insurance plans, studies, ...) and may be used to assist with indexing and searching for appropriate evidence instances.</t>
@@ -671,10 +671,10 @@
 </t>
   </si>
   <si>
-    <t>Link to artifact associated with summary</t>
-  </si>
-  <si>
-    <t>Link to artifact associated with summary.</t>
+    <t>Link or citation to artifact associated with the summary</t>
+  </si>
+  <si>
+    <t>Link or citation to artifact associated with the summary.</t>
   </si>
   <si>
     <t>Evidence.description</t>
@@ -763,7 +763,10 @@
     <t>Evidence.population.description</t>
   </si>
   <si>
-    <t>Description of the particular summary.</t>
+    <t>Textual description of population</t>
+  </si>
+  <si>
+    <t>Textual description of population.</t>
   </si>
   <si>
     <t>Evidence.population.note</t>
@@ -776,10 +779,10 @@
 </t>
   </si>
   <si>
-    <t>The evidence that the summary indirectly represents</t>
-  </si>
-  <si>
-    <t>The evidence that the summary indirectly represents.</t>
+    <t>Descriptive (not actual) expression of the population this evidence is about, eg inclusion criteria for research study</t>
+  </si>
+  <si>
+    <t>Descriptive (not actual) expression of the population this evidence is about, eg inclusion criteria for research study.</t>
   </si>
   <si>
     <t>Evidence.population.sampleCohort</t>
@@ -789,10 +792,10 @@
 </t>
   </si>
   <si>
-    <t>The evidence from which the sample was drawn</t>
-  </si>
-  <si>
-    <t>The evidence from which the sample was drawn.</t>
+    <t>Summary statistics describing the actual group for this population</t>
+  </si>
+  <si>
+    <t>Summary statistics describing the actual group for this population.</t>
   </si>
   <si>
     <t>The target reference must conform to the CohortSummary profile.</t>
@@ -801,19 +804,19 @@
     <t>Evidence.population.actualCohort</t>
   </si>
   <si>
-    <t>The evidence that the summary directly reprresents</t>
-  </si>
-  <si>
-    <t>The evidence that the summary directly reprresents.</t>
+    <t>The actual group (ie list of members) for this population</t>
+  </si>
+  <si>
+    <t>The actual group (ie list of members) for this population.</t>
   </si>
   <si>
     <t>Evidence.population.sampleSize</t>
   </si>
   <si>
-    <t>Sample description</t>
-  </si>
-  <si>
-    <t>Sample description.</t>
+    <t>Sample size for the population</t>
+  </si>
+  <si>
+    <t>Sample size for the population.</t>
   </si>
   <si>
     <t>Evidence.population.sampleSize.id</t>
@@ -828,10 +831,10 @@
     <t>Evidence.population.sampleSize.description</t>
   </si>
   <si>
-    <t>Description of the sample size</t>
-  </si>
-  <si>
-    <t>Description of the sample size.</t>
+    <t>Textual description of population sample</t>
+  </si>
+  <si>
+    <t>Textual description of population sample.</t>
   </si>
   <si>
     <t>Evidence.population.sampleSize.note</t>
@@ -911,19 +914,19 @@
 </t>
   </si>
   <si>
-    <t>The definition of a nested variable</t>
-  </si>
-  <si>
-    <t>The definition of a nested variable.</t>
+    <t>Definition of a variable related to the statistic(s)</t>
+  </si>
+  <si>
+    <t>Definition of a variable related to the statistic(s).</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.statisticCollection</t>
   </si>
   <si>
-    <t>Set of statistics associated with variable</t>
-  </si>
-  <si>
-    <t>Set of statistics associated with variable.</t>
+    <t>Set of statistics</t>
+  </si>
+  <si>
+    <t>Set of statistics.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.statisticCollection.id</t>
@@ -938,22 +941,16 @@
     <t>Evidence.population.evidenceVariable.statisticCollection.description</t>
   </si>
   <si>
-    <t>Description of statistic</t>
-  </si>
-  <si>
-    <t>Description of statistic.</t>
+    <t>Textual description related to the set of statistics</t>
+  </si>
+  <si>
+    <t>Textual description related to the set of statistics.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.statisticCollection.note</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.statisticCollection.synthesisType</t>
-  </si>
-  <si>
-    <t>The type of synthesis statistic</t>
-  </si>
-  <si>
-    <t>The type of synthesis statistic.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.statisticCollection.studyType</t>
@@ -972,32 +969,32 @@
 </t>
   </si>
   <si>
-    <t>The statistic value(s)</t>
-  </si>
-  <si>
-    <t>The statistic value(s).</t>
-  </si>
-  <si>
-    <t>Evidence.population.evidenceVariable.distribution</t>
+    <t>Values and parameters for a single statistic</t>
+  </si>
+  <si>
+    <t>Values and parameters for a single statistic.</t>
+  </si>
+  <si>
+    <t>Evidence.population.evidenceVariable.statisticCollection.distribution</t>
   </si>
   <si>
     <t xml:space="preserve">OrderedDistribution
 </t>
   </si>
   <si>
-    <t>Ordered distribution</t>
-  </si>
-  <si>
-    <t>Ordered distribution.</t>
+    <t>An ordered group of statistics</t>
+  </si>
+  <si>
+    <t>An ordered group of statistics.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.nestedVariable</t>
   </si>
   <si>
-    <t>Dependent evvidence variable</t>
-  </si>
-  <si>
-    <t>Dependent evvidence variable.</t>
+    <t>An evidence variable, nested for denoting that statistics relate to both this variable and the previously noted variable</t>
+  </si>
+  <si>
+    <t>An evidence variable, nested for denoting that statistics relate to both this variable and the previously noted variable.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.nestedVariable.id</t>
@@ -1048,10 +1045,10 @@
     <t>Evidence.population.evidenceVariable.nestedVariable.statisticCollection.additionalVariable</t>
   </si>
   <si>
-    <t>Additional variables</t>
-  </si>
-  <si>
-    <t>Additional variables.</t>
+    <t>An evidence variable, nested for denoting that statistics relate to this variable, any additional variables, plus the two previously noted variables</t>
+  </si>
+  <si>
+    <t>An evidence variable, nested for denoting that statistics relate to this variable, any additional variables, plus the two previously noted variables.</t>
   </si>
   <si>
     <t>Evidence.population.evidenceVariable.nestedVariable.statisticCollection.additionalVariable.id</t>
@@ -1069,13 +1066,10 @@
     <t>Evidence.population.evidenceVariable.nestedVariable.statisticCollection.additionalVariable.variableDefinition</t>
   </si>
   <si>
-    <t>Definition of additional variable</t>
-  </si>
-  <si>
-    <t>Definition of additional variable.</t>
-  </si>
-  <si>
     <t>Evidence.population.evidenceVariable.nestedVariable.statisticCollection.statistic</t>
+  </si>
+  <si>
+    <t>Evidence.population.evidenceVariable.nestedVariable.statisticCollection.distribution</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1203,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM92"/>
+  <dimension ref="A1:AM93"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1228,7 +1222,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="67.43359375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="128.2421875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -5497,10 +5491,10 @@
         <v>162</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -5580,7 +5574,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5660,7 +5654,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -5689,7 +5683,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5712,13 +5706,13 @@
         <v>40</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5769,7 +5763,7 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>41</v>
@@ -5798,7 +5792,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5821,16 +5815,16 @@
         <v>40</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -5880,7 +5874,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -5909,7 +5903,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5932,13 +5926,13 @@
         <v>40</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5989,7 +5983,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6018,7 +6012,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6044,10 +6038,10 @@
         <v>180</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6098,7 +6092,7 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -6127,7 +6121,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6236,7 +6230,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6347,7 +6341,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6460,7 +6454,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6486,10 +6480,10 @@
         <v>119</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6540,7 +6534,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6569,7 +6563,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6649,7 +6643,7 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -6678,7 +6672,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6701,13 +6695,13 @@
         <v>40</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6758,7 +6752,7 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -6787,7 +6781,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6810,13 +6804,13 @@
         <v>40</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -6867,7 +6861,7 @@
         <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -6896,7 +6890,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6922,10 +6916,10 @@
         <v>180</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6976,7 +6970,7 @@
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7005,7 +6999,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7114,7 +7108,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7225,7 +7219,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7338,7 +7332,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7364,10 +7358,10 @@
         <v>162</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7418,7 +7412,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7447,7 +7441,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7527,7 +7521,7 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7556,7 +7550,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7582,10 +7576,10 @@
         <v>67</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7615,10 +7609,10 @@
         <v>140</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>40</v>
@@ -7636,7 +7630,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7665,7 +7659,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7688,13 +7682,13 @@
         <v>49</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7745,7 +7739,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>48</v>
@@ -7774,7 +7768,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7800,10 +7794,10 @@
         <v>180</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -7854,7 +7848,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -7883,7 +7877,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -7992,7 +7986,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8103,7 +8097,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8216,7 +8210,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8242,10 +8236,10 @@
         <v>162</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8296,7 +8290,7 @@
         <v>40</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>41</v>
@@ -8325,7 +8319,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8405,7 +8399,7 @@
         <v>40</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>41</v>
@@ -8434,7 +8428,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8460,10 +8454,10 @@
         <v>222</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>302</v>
+        <v>224</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -8514,7 +8508,7 @@
         <v>40</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>41</v>
@@ -8543,7 +8537,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8569,10 +8563,10 @@
         <v>222</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -8623,7 +8617,7 @@
         <v>40</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>41</v>
@@ -8652,7 +8646,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -8675,13 +8669,13 @@
         <v>49</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8732,7 +8726,7 @@
         <v>40</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>48</v>
@@ -8761,7 +8755,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -8784,13 +8778,13 @@
         <v>40</v>
       </c>
       <c r="J69" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K69" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="K69" t="s" s="2">
+      <c r="L69" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -8841,7 +8835,7 @@
         <v>40</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>41</v>
@@ -8870,7 +8864,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -8896,10 +8890,10 @@
         <v>180</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>315</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>316</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -8950,7 +8944,7 @@
         <v>40</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>41</v>
@@ -8979,7 +8973,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9088,7 +9082,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9199,7 +9193,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9312,7 +9306,7 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9338,10 +9332,10 @@
         <v>162</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -9392,7 +9386,7 @@
         <v>40</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>41</v>
@@ -9421,7 +9415,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9501,7 +9495,7 @@
         <v>40</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>41</v>
@@ -9530,7 +9524,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9556,10 +9550,10 @@
         <v>67</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -9589,10 +9583,10 @@
         <v>140</v>
       </c>
       <c r="X76" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y76" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Z76" t="s" s="2">
         <v>40</v>
@@ -9610,7 +9604,7 @@
         <v>40</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>41</v>
@@ -9639,7 +9633,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9662,13 +9656,13 @@
         <v>49</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -9719,7 +9713,7 @@
         <v>40</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>48</v>
@@ -9748,7 +9742,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -9774,10 +9768,10 @@
         <v>180</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -9828,7 +9822,7 @@
         <v>40</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>41</v>
@@ -9857,7 +9851,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -9966,7 +9960,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10077,7 +10071,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10190,7 +10184,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10216,10 +10210,10 @@
         <v>162</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -10270,7 +10264,7 @@
         <v>40</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>41</v>
@@ -10299,7 +10293,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -10379,7 +10373,7 @@
         <v>40</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>41</v>
@@ -10408,7 +10402,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10434,10 +10428,10 @@
         <v>222</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>302</v>
+        <v>224</v>
       </c>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -10488,7 +10482,7 @@
         <v>40</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>41</v>
@@ -10517,7 +10511,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10543,10 +10537,10 @@
         <v>222</v>
       </c>
       <c r="K85" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="L85" t="s" s="2">
         <v>304</v>
-      </c>
-      <c r="L85" t="s" s="2">
-        <v>305</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -10597,7 +10591,7 @@
         <v>40</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>41</v>
@@ -10626,7 +10620,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10652,10 +10646,10 @@
         <v>180</v>
       </c>
       <c r="K86" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="L86" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="L86" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -10706,7 +10700,7 @@
         <v>40</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>41</v>
@@ -10735,7 +10729,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -10844,7 +10838,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -10955,7 +10949,7 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11068,7 +11062,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11094,10 +11088,10 @@
         <v>67</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -11127,10 +11121,10 @@
         <v>140</v>
       </c>
       <c r="X90" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Z90" t="s" s="2">
         <v>40</v>
@@ -11148,7 +11142,7 @@
         <v>40</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>41</v>
@@ -11177,7 +11171,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11200,13 +11194,13 @@
         <v>49</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>340</v>
+        <v>289</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>341</v>
+        <v>290</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -11257,7 +11251,7 @@
         <v>40</v>
       </c>
       <c r="AE91" t="s" s="2">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AF91" t="s" s="2">
         <v>48</v>
@@ -11286,7 +11280,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -11309,13 +11303,13 @@
         <v>49</v>
       </c>
       <c r="J92" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="K92" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="K92" t="s" s="2">
+      <c r="L92" t="s" s="2">
         <v>308</v>
-      </c>
-      <c r="L92" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -11366,7 +11360,7 @@
         <v>40</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>48</v>
@@ -11390,6 +11384,115 @@
         <v>40</v>
       </c>
       <c r="AM92" t="s" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="F93" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="H93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="I93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="J93" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K93" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="R93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="S93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="T93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE93" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="AF93" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG93" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AH93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM93" t="s" s="2">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed datatypes and removed EvidenceSet
</commit_message>
<xml_diff>
--- a/image/evidence.xlsx
+++ b/image/evidence.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2147" uniqueCount="300">
   <si>
     <t>Path</t>
   </si>
@@ -670,21 +670,17 @@
     <t>Evidence.referentGroup.evidenceSource</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Group|EvidenceSet)
-</t>
-  </si>
-  <si>
-    <t>Various information categories of group</t>
-  </si>
-  <si>
-    <t>Various information categories of group.</t>
-  </si>
-  <si>
-    <t>Evidence.referentGroup.intendedGroup</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference(Group)
 </t>
+  </si>
+  <si>
+    <t>Various information categories of group</t>
+  </si>
+  <si>
+    <t>Various information categories of group.</t>
+  </si>
+  <si>
+    <t>Evidence.referentGroup.intendedGroup</t>
   </si>
   <si>
     <t>Non-actual group that is a set of characteristics</t>
@@ -4594,13 +4590,13 @@
         <v>40</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="K32" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="K32" t="s" s="2">
+      <c r="L32" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>216</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -4680,7 +4676,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4703,13 +4699,13 @@
         <v>40</v>
       </c>
       <c r="J33" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="K33" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="K33" t="s" s="2">
+      <c r="L33" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -4736,14 +4732,14 @@
         <v>40</v>
       </c>
       <c r="W33" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="X33" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="X33" t="s" s="2">
+      <c r="Y33" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="Y33" t="s" s="2">
-        <v>223</v>
-      </c>
       <c r="Z33" t="s" s="2">
         <v>40</v>
       </c>
@@ -4760,7 +4756,7 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -4789,7 +4785,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4815,10 +4811,10 @@
         <v>188</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>225</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>226</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -4869,7 +4865,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -4898,7 +4894,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5007,7 +5003,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5118,7 +5114,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5231,7 +5227,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5257,10 +5253,10 @@
         <v>175</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5311,7 +5307,7 @@
         <v>40</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>41</v>
@@ -5340,7 +5336,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5420,7 +5416,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5449,7 +5445,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5472,13 +5468,13 @@
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>235</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>236</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -5505,14 +5501,14 @@
         <v>40</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X40" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="Y40" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="Y40" t="s" s="2">
-        <v>238</v>
-      </c>
       <c r="Z40" t="s" s="2">
         <v>40</v>
       </c>
@@ -5529,7 +5525,7 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>41</v>
@@ -5558,7 +5554,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5581,13 +5577,13 @@
         <v>49</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>242</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5638,7 +5634,7 @@
         <v>40</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>48</v>
@@ -5667,7 +5663,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -5690,13 +5686,13 @@
         <v>40</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -5747,7 +5743,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -5776,7 +5772,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -5799,13 +5795,13 @@
         <v>40</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="K43" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="K43" t="s" s="2">
-        <v>219</v>
-      </c>
       <c r="L43" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -5832,14 +5828,14 @@
         <v>40</v>
       </c>
       <c r="W43" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="X43" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="X43" t="s" s="2">
+      <c r="Y43" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="Y43" t="s" s="2">
-        <v>223</v>
-      </c>
       <c r="Z43" t="s" s="2">
         <v>40</v>
       </c>
@@ -5856,7 +5852,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -5885,7 +5881,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -5908,13 +5904,13 @@
         <v>40</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>249</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>250</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -5941,14 +5937,14 @@
         <v>40</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X44" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="Y44" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="Y44" t="s" s="2">
-        <v>252</v>
-      </c>
       <c r="Z44" t="s" s="2">
         <v>40</v>
       </c>
@@ -5965,7 +5961,7 @@
         <v>40</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>41</v>
@@ -5994,7 +5990,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6017,13 +6013,13 @@
         <v>40</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="L45" t="s" s="2">
         <v>254</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6050,14 +6046,14 @@
         <v>40</v>
       </c>
       <c r="W45" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X45" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y45" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="Y45" t="s" s="2">
-        <v>257</v>
-      </c>
       <c r="Z45" t="s" s="2">
         <v>40</v>
       </c>
@@ -6074,7 +6070,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6103,7 +6099,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6126,13 +6122,13 @@
         <v>40</v>
       </c>
       <c r="J46" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="K46" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="K46" t="s" s="2">
+      <c r="L46" t="s" s="2">
         <v>260</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>261</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -6183,7 +6179,7 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6212,7 +6208,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6235,13 +6231,13 @@
         <v>40</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="K47" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="L47" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>265</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6292,7 +6288,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6321,7 +6317,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6347,10 +6343,10 @@
         <v>188</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>268</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6401,7 +6397,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6430,7 +6426,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6539,7 +6535,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6650,7 +6646,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6763,7 +6759,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -6789,10 +6785,10 @@
         <v>119</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6843,7 +6839,7 @@
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -6872,7 +6868,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -6952,7 +6948,7 @@
         <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -6981,7 +6977,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7004,13 +7000,13 @@
         <v>40</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>277</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>278</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7037,14 +7033,14 @@
         <v>40</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X54" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="Y54" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="Y54" t="s" s="2">
-        <v>280</v>
-      </c>
       <c r="Z54" t="s" s="2">
         <v>40</v>
       </c>
@@ -7061,7 +7057,7 @@
         <v>40</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>41</v>
@@ -7090,7 +7086,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7116,10 +7112,10 @@
         <v>188</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>283</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7170,7 +7166,7 @@
         <v>40</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>41</v>
@@ -7199,7 +7195,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7308,7 +7304,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7419,7 +7415,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7532,7 +7528,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7558,10 +7554,10 @@
         <v>119</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -7612,7 +7608,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -7641,7 +7637,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7667,10 +7663,10 @@
         <v>184</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>291</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>292</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -7721,7 +7717,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -7750,7 +7746,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -7773,7 +7769,7 @@
         <v>40</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K61" t="s" s="2">
         <v>185</v>
@@ -7806,14 +7802,14 @@
         <v>40</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="Y61" t="s" s="2">
-        <v>295</v>
-      </c>
       <c r="Z61" t="s" s="2">
         <v>40</v>
       </c>
@@ -7830,7 +7826,7 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -7859,7 +7855,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -7882,13 +7878,13 @@
         <v>40</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -7915,14 +7911,14 @@
         <v>40</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="Y62" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="Y62" t="s" s="2">
-        <v>300</v>
-      </c>
       <c r="Z62" t="s" s="2">
         <v>40</v>
       </c>
@@ -7939,7 +7935,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
Deleted ResearchDefinition & ResearchElementDefinition
</commit_message>
<xml_diff>
--- a/image/evidence.xlsx
+++ b/image/evidence.xlsx
@@ -4466,7 +4466,7 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>48</v>
@@ -4478,7 +4478,7 @@
         <v>40</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="J31" t="s" s="2">
         <v>210</v>
@@ -4541,7 +4541,7 @@
         <v>209</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>48</v>

</xml_diff>